<commit_message>
Add the column of dislikes
</commit_message>
<xml_diff>
--- a/data/서울신문_전세계아프간난민딜레마.xlsx
+++ b/data/서울신문_전세계아프간난민딜레마.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E287"/>
+  <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>추천수</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>비추천수</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -479,6 +484,11 @@
           <t>1460</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -504,6 +514,11 @@
           <t>968</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -529,6 +544,11 @@
           <t>715</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -554,6 +574,11 @@
           <t>270</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -579,6 +604,11 @@
           <t>193</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -604,6 +634,11 @@
           <t>123</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -629,6 +664,11 @@
           <t>104</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -654,6 +694,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -679,6 +724,11 @@
           <t>86</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -704,6 +754,11 @@
           <t>84</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -729,6 +784,11 @@
           <t>82</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -754,6 +814,11 @@
           <t>81</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -779,6 +844,11 @@
           <t>69</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -804,6 +874,11 @@
           <t>55</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -829,6 +904,11 @@
           <t>37</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -854,6 +934,11 @@
           <t>37</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -879,6 +964,11 @@
           <t>35</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -904,6 +994,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -929,6 +1024,11 @@
           <t>27</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -954,6 +1054,11 @@
           <t>25</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -979,6 +1084,11 @@
           <t>24</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1004,6 +1114,11 @@
           <t>24</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1029,6 +1144,11 @@
           <t>20</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1054,6 +1174,11 @@
           <t>20</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1079,6 +1204,11 @@
           <t>18</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1104,6 +1234,11 @@
           <t>16</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1129,6 +1264,11 @@
           <t>16</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1154,6 +1294,11 @@
           <t>16</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1179,6 +1324,11 @@
           <t>15</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1204,6 +1354,11 @@
           <t>13</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1229,6 +1384,11 @@
           <t>13</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1254,6 +1414,11 @@
           <t>12</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1279,6 +1444,11 @@
           <t>11</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1304,6 +1474,11 @@
           <t>11</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1329,6 +1504,11 @@
           <t>11</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1354,6 +1534,11 @@
           <t>11</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1379,6 +1564,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1404,6 +1594,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1429,6 +1624,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1454,6 +1654,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1479,6 +1684,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1504,6 +1714,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1529,6 +1744,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1554,6 +1774,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1579,6 +1804,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1604,6 +1834,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1629,6 +1864,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1654,6 +1894,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1679,6 +1924,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1704,6 +1954,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1729,6 +1984,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1754,6 +2014,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1779,6 +2044,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1804,6 +2074,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1829,6 +2104,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1854,6 +2134,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1879,6 +2164,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1904,6 +2194,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1929,6 +2224,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1954,6 +2254,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1979,6 +2284,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2004,6 +2314,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2029,6 +2344,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2054,6 +2374,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2079,6 +2404,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2104,6 +2434,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2129,6 +2464,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2154,6 +2494,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2179,6 +2524,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2204,6 +2554,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2229,6 +2584,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2254,6 +2614,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2279,6 +2644,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2304,6 +2674,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2329,6 +2704,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2354,6 +2734,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2379,6 +2764,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2404,6 +2794,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2429,6 +2824,11 @@
           <t>7</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2454,6 +2854,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2479,6 +2884,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2504,6 +2914,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2529,6 +2944,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2554,6 +2974,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2579,6 +3004,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2604,6 +3034,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2629,6 +3064,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2654,6 +3094,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2679,6 +3124,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2704,6 +3154,11 @@
           <t>4</t>
         </is>
       </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2729,6 +3184,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2754,6 +3214,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2779,6 +3244,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2804,6 +3274,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2829,6 +3304,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2854,6 +3334,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2879,6 +3364,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2904,6 +3394,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2929,6 +3424,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2954,6 +3454,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2979,6 +3484,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3004,6 +3514,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3029,6 +3544,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3054,6 +3574,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3079,6 +3604,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3104,6 +3634,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3129,6 +3664,11 @@
           <t>5</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3154,6 +3694,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3179,6 +3724,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3204,6 +3754,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3229,6 +3784,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3254,6 +3814,11 @@
           <t>3</t>
         </is>
       </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -3279,6 +3844,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -3304,6 +3874,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -3329,6 +3904,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -3354,6 +3934,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -3379,6 +3964,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -3404,6 +3994,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -3429,6 +4024,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -3454,6 +4054,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -3479,6 +4084,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -3504,6 +4114,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -3529,6 +4144,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -3554,6 +4174,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -3579,6 +4204,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -3604,6 +4234,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -3629,6 +4264,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -3654,6 +4294,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -3679,6 +4324,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -3704,6 +4354,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -3729,6 +4384,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -3754,6 +4414,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -3779,6 +4444,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -3804,6 +4474,11 @@
           <t>6</t>
         </is>
       </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -3829,6 +4504,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -3854,6 +4534,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -3879,6 +4564,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -3904,6 +4594,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -3929,6 +4624,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -3954,6 +4654,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -3979,6 +4684,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -4004,6 +4714,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -4029,6 +4744,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -4054,6 +4774,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4079,6 +4804,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -4104,6 +4834,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -4129,6 +4864,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -4154,6 +4894,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -4179,6 +4924,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -4204,6 +4954,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -4229,6 +4984,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -4254,6 +5014,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -4279,6 +5044,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -4304,6 +5074,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -4329,6 +5104,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -4354,6 +5134,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -4379,6 +5164,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -4404,6 +5194,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -4429,6 +5224,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -4454,6 +5254,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -4479,6 +5284,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -4504,6 +5314,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -4529,6 +5344,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -4554,6 +5374,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -4579,6 +5404,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -4604,6 +5434,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -4629,6 +5464,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -4654,6 +5494,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -4679,6 +5524,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -4704,6 +5554,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -4729,6 +5584,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -4754,6 +5614,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -4779,6 +5644,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -4804,6 +5674,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -4829,6 +5704,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -4854,6 +5734,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -4879,6 +5764,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -4904,6 +5794,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -4929,6 +5824,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -4954,6 +5854,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -4979,6 +5884,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -5004,6 +5914,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -5029,6 +5944,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -5054,6 +5974,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -5079,6 +6004,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -5104,6 +6034,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -5129,6 +6064,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -5154,6 +6094,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -5179,6 +6124,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -5204,6 +6154,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -5229,6 +6184,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -5254,6 +6214,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -5279,6 +6244,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -5304,6 +6274,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -5329,6 +6304,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -5354,6 +6334,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -5379,6 +6364,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -5404,6 +6394,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -5429,6 +6424,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -5454,6 +6454,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -5479,6 +6484,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -5504,6 +6514,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -5529,6 +6544,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -5554,6 +6574,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -5579,6 +6604,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -5604,6 +6634,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -5629,6 +6664,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -5654,6 +6694,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -5679,6 +6724,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -5704,6 +6754,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -5729,6 +6784,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -5754,6 +6814,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -5779,6 +6844,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -5804,6 +6874,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -5829,6 +6904,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -5854,6 +6934,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -5879,6 +6964,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -5904,6 +6994,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -5929,6 +7024,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -5954,6 +7054,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -5979,6 +7084,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -6004,6 +7114,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -6029,6 +7144,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -6054,6 +7174,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -6079,6 +7204,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -6104,6 +7234,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -6129,6 +7264,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -6154,6 +7294,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -6179,6 +7324,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -6204,6 +7354,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -6229,6 +7384,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -6254,6 +7414,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -6279,6 +7444,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -6304,6 +7474,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -6329,6 +7504,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -6354,6 +7534,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -6379,6 +7564,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -6404,6 +7594,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -6429,6 +7624,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -6454,6 +7654,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -6479,6 +7684,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -6504,6 +7714,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -6529,6 +7744,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -6554,6 +7774,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -6579,6 +7804,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -6604,6 +7834,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -6629,6 +7864,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -6654,6 +7894,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -6679,6 +7924,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -6704,6 +7954,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -6729,6 +7984,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -6754,6 +8014,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -6779,6 +8044,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -6804,6 +8074,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -6829,6 +8104,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -6854,6 +8134,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -6879,6 +8164,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -6904,6 +8194,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -6929,6 +8224,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -6954,6 +8254,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -6979,6 +8284,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -7004,6 +8314,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -7029,6 +8344,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -7054,6 +8374,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -7079,6 +8404,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -7104,6 +8434,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -7129,6 +8464,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -7154,6 +8494,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -7179,6 +8524,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -7204,6 +8554,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -7229,6 +8584,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -7254,6 +8614,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -7279,6 +8644,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -7304,6 +8674,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -7329,6 +8704,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -7354,6 +8734,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -7379,6 +8764,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -7404,6 +8794,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -7429,6 +8824,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -7454,6 +8854,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -7479,6 +8884,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -7504,6 +8914,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -7529,6 +8944,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -7554,6 +8974,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -7579,6 +9004,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -7602,6 +9032,11 @@
       <c r="E287" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>17</t>
         </is>
       </c>
     </row>

</xml_diff>